<commit_message>
Correcciones a la lista de ratings.
</commit_message>
<xml_diff>
--- a/TP_Final/TEXTO/Rating.xlsx
+++ b/TP_Final/TEXTO/Rating.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakaneko\Facultad\Materias\Circuitos Electrónicos II\TPS\REPO-TPS\Circuitos-2\TP_Final\TEXTO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="11715" windowHeight="6210"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="11715" windowHeight="6210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Transistores" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="463">
   <si>
     <t>Ref.</t>
   </si>
@@ -1319,36 +1324,18 @@
     <t>16V</t>
   </si>
   <si>
-    <t>10V</t>
-  </si>
-  <si>
     <t>Electrolítico</t>
   </si>
   <si>
     <t>Cerámico</t>
   </si>
   <si>
-    <t>100VAC</t>
-  </si>
-  <si>
-    <t>50VAC</t>
-  </si>
-  <si>
-    <t>80VAC</t>
-  </si>
-  <si>
-    <t>Cerámico / Tantalio</t>
-  </si>
-  <si>
     <t>100V</t>
   </si>
   <si>
     <t>50V</t>
   </si>
   <si>
-    <t>10VAC</t>
-  </si>
-  <si>
     <t>Tensión Máxima3</t>
   </si>
   <si>
@@ -1401,12 +1388,36 @@
   </si>
   <si>
     <t>1/2</t>
+  </si>
+  <si>
+    <t>Alambre cementada</t>
+  </si>
+  <si>
+    <t>Carbón/Metal Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bourns vertical 25 vueltas</t>
+  </si>
+  <si>
+    <t>Bourns vertical 25 vueltas</t>
+  </si>
+  <si>
+    <t>Cerámico /Polyester</t>
+  </si>
+  <si>
+    <t>Cerámico/Polyester</t>
+  </si>
+  <si>
+    <t>35V</t>
+  </si>
+  <si>
+    <t>SyC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2069,6 +2080,16 @@
   </cellStyles>
   <dxfs count="32">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2088,10 +2109,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2236,22 +2263,6 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2275,37 +2286,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:O29" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:O29" totalsRowShown="0" headerRowDxfId="31">
   <autoFilter ref="A1:O29"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Referencia"/>
-    <tableColumn id="2" name="Fabricante" dataDxfId="25"/>
+    <tableColumn id="2" name="Fabricante" dataDxfId="30"/>
     <tableColumn id="3" name="Modelo"/>
-    <tableColumn id="4" name="Tipo" dataDxfId="24"/>
+    <tableColumn id="4" name="Tipo" dataDxfId="29"/>
     <tableColumn id="5" name="Función"/>
-    <tableColumn id="6" name="Corriente RMS" dataDxfId="23"/>
-    <tableColumn id="7" name="Corriente Máxima" dataDxfId="22"/>
-    <tableColumn id="8" name="Tensión Máxima" dataDxfId="21"/>
-    <tableColumn id="9" name="Potencia Media" dataDxfId="20"/>
-    <tableColumn id="10" name="Potencia Máxima" dataDxfId="19"/>
-    <tableColumn id="11" name="Rating Maximos absolutos" dataDxfId="18"/>
-    <tableColumn id="12" name="Encapsulado" dataDxfId="17"/>
-    <tableColumn id="13" name="Montaje" dataDxfId="16"/>
-    <tableColumn id="14" name="Proveedor" dataDxfId="15"/>
-    <tableColumn id="15" name="Precio" dataDxfId="14"/>
+    <tableColumn id="6" name="Corriente RMS" dataDxfId="28"/>
+    <tableColumn id="7" name="Corriente Máxima" dataDxfId="27"/>
+    <tableColumn id="8" name="Tensión Máxima" dataDxfId="26"/>
+    <tableColumn id="9" name="Potencia Media" dataDxfId="25"/>
+    <tableColumn id="10" name="Potencia Máxima" dataDxfId="24"/>
+    <tableColumn id="11" name="Rating Maximos absolutos" dataDxfId="23"/>
+    <tableColumn id="12" name="Encapsulado" dataDxfId="22"/>
+    <tableColumn id="13" name="Montaje" dataDxfId="21"/>
+    <tableColumn id="14" name="Proveedor" dataDxfId="20"/>
+    <tableColumn id="15" name="Precio" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Capacitores" displayName="Capacitores" ref="A1:F26" totalsRowShown="0" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Capacitores" displayName="Capacitores" ref="A1:F26" totalsRowShown="0" tableBorderDxfId="18">
   <autoFilter ref="A1:F26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Ref." dataDxfId="12"/>
-    <tableColumn id="2" name="Description" dataDxfId="11"/>
-    <tableColumn id="3" name="Valor" dataDxfId="10"/>
-    <tableColumn id="4" name="Tensión Máxima" dataDxfId="9"/>
+    <tableColumn id="1" name="Ref." dataDxfId="17"/>
+    <tableColumn id="2" name="Description" dataDxfId="16"/>
+    <tableColumn id="3" name="Valor" dataDxfId="15"/>
+    <tableColumn id="4" name="Tensión Máxima" dataDxfId="14"/>
     <tableColumn id="5" name="Tensión de Operación"/>
     <tableColumn id="6" name="Tensión Máxima3"/>
   </tableColumns>
@@ -2318,15 +2329,15 @@
   <autoFilter ref="A1:J21"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Ref"/>
-    <tableColumn id="2" name="Modelo" dataDxfId="8"/>
-    <tableColumn id="4" name="Tensión Máxima" dataDxfId="6"/>
-    <tableColumn id="5" name="Corriente Máxima" dataDxfId="7"/>
-    <tableColumn id="6" name="Potencia Máxima" dataDxfId="31"/>
-    <tableColumn id="7" name="Potencia Promedio" dataDxfId="30"/>
-    <tableColumn id="3" name="Encapsulado" dataDxfId="5"/>
-    <tableColumn id="8" name="Montaje" dataDxfId="4"/>
-    <tableColumn id="9" name="Proveedor" dataDxfId="3"/>
-    <tableColumn id="10" name="Precio" dataDxfId="2"/>
+    <tableColumn id="2" name="Modelo" dataDxfId="13"/>
+    <tableColumn id="4" name="Tensión Máxima" dataDxfId="12"/>
+    <tableColumn id="5" name="Corriente Máxima" dataDxfId="11"/>
+    <tableColumn id="6" name="Potencia Máxima" dataDxfId="10"/>
+    <tableColumn id="7" name="Potencia Promedio" dataDxfId="9"/>
+    <tableColumn id="3" name="Encapsulado" dataDxfId="8"/>
+    <tableColumn id="8" name="Montaje" dataDxfId="7"/>
+    <tableColumn id="9" name="Proveedor" dataDxfId="6"/>
+    <tableColumn id="10" name="Precio" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2337,8 +2348,8 @@
   <autoFilter ref="A1:E44"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ref"/>
-    <tableColumn id="2" name="Valor" dataDxfId="1"/>
-    <tableColumn id="3" name="Potencia Media" dataDxfId="0"/>
+    <tableColumn id="2" name="Valor" dataDxfId="4"/>
+    <tableColumn id="3" name="Potencia Media" dataDxfId="3"/>
     <tableColumn id="4" name="Disipación de Potencia [W]"/>
     <tableColumn id="5" name="Tecnología"/>
   </tableColumns>
@@ -2350,8 +2361,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A1:B7" totalsRowShown="0">
   <autoFilter ref="A1:B7"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Ref" dataDxfId="29"/>
-    <tableColumn id="2" name="Potencia Promedio" dataDxfId="28"/>
+    <tableColumn id="1" name="Ref" dataDxfId="2"/>
+    <tableColumn id="2" name="Potencia Promedio" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2362,14 +2373,14 @@
   <autoFilter ref="E1:F6"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Columna1"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="27"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2411,7 +2422,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2446,7 +2457,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2657,11 +2668,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
@@ -4040,10 +4051,10 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
@@ -4070,7 +4081,7 @@
         <v>431</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4090,7 +4101,7 @@
         <v>432</v>
       </c>
       <c r="F2" s="84" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4107,10 +4118,10 @@
         <v>1.5</v>
       </c>
       <c r="E3" s="82" t="s">
-        <v>442</v>
+        <v>461</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4127,10 +4138,10 @@
         <v>329</v>
       </c>
       <c r="E4" s="108" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="F4" s="108" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4147,10 +4158,10 @@
         <v>330</v>
       </c>
       <c r="E5" s="144" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="F5" s="145" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4167,10 +4178,10 @@
         <v>331</v>
       </c>
       <c r="E6" s="136" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F6" s="136" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4187,10 +4198,10 @@
         <v>332</v>
       </c>
       <c r="E7" s="136" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F7" s="136" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4207,10 +4218,10 @@
         <v>333</v>
       </c>
       <c r="E8" s="140" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F8" s="140" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4227,10 +4238,10 @@
         <v>334</v>
       </c>
       <c r="E9" s="140" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F9" s="140" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4247,10 +4258,10 @@
         <v>335</v>
       </c>
       <c r="E10" s="147" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F10" s="147" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4267,10 +4278,10 @@
         <v>323</v>
       </c>
       <c r="E11" s="110" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F11" s="110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4287,10 +4298,10 @@
         <v>324</v>
       </c>
       <c r="E12" s="110" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F12" s="86" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4307,10 +4318,10 @@
         <v>325</v>
       </c>
       <c r="E13" s="110" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F13" s="110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4327,10 +4338,10 @@
         <v>326</v>
       </c>
       <c r="E14" s="110" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F14" s="86" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4347,10 +4358,10 @@
         <v>323</v>
       </c>
       <c r="E15" s="112" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F15" s="112" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4367,10 +4378,10 @@
         <v>324</v>
       </c>
       <c r="E16" s="112" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F16" s="114" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4387,10 +4398,10 @@
         <v>325</v>
       </c>
       <c r="E17" s="112" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F17" s="112" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4407,10 +4418,10 @@
         <v>326</v>
       </c>
       <c r="E18" s="114" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F18" s="114" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4427,10 +4438,10 @@
         <v>327</v>
       </c>
       <c r="E19" s="110" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F19" s="110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4447,10 +4458,10 @@
         <v>328</v>
       </c>
       <c r="E20" s="86" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F20" s="110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4467,10 +4478,10 @@
         <v>327</v>
       </c>
       <c r="E21" s="112" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F21" s="114" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4487,10 +4498,10 @@
         <v>328</v>
       </c>
       <c r="E22" s="114" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F22" s="114" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4510,7 +4521,7 @@
         <v>432</v>
       </c>
       <c r="F23" s="78" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4530,7 +4541,7 @@
         <v>432</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4547,10 +4558,10 @@
         <v>337</v>
       </c>
       <c r="E25" s="112" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="F25" s="112" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4567,10 +4578,10 @@
         <v>338</v>
       </c>
       <c r="E26" s="114" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="F26" s="114" t="s">
-        <v>439</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -4586,11 +4597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -4652,13 +4663,13 @@
         <v>286</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>406</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="J2" s="35">
         <v>90</v>
@@ -4684,13 +4695,13 @@
         <v>289</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="H3" s="35" t="s">
         <v>406</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="J3" s="35">
         <v>90</v>
@@ -4716,13 +4727,13 @@
         <v>294</v>
       </c>
       <c r="G4" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H4" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I4" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J4" s="106">
         <v>4</v>
@@ -4748,13 +4759,13 @@
         <v>297</v>
       </c>
       <c r="G5" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H5" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I5" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J5" s="106">
         <v>4</v>
@@ -4776,13 +4787,13 @@
         <v>396</v>
       </c>
       <c r="G6" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H6" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I6" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J6" s="106">
         <v>4</v>
@@ -4804,13 +4815,13 @@
         <v>396</v>
       </c>
       <c r="G7" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H7" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I7" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J7" s="106">
         <v>4</v>
@@ -4832,13 +4843,13 @@
         <v>396</v>
       </c>
       <c r="G8" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H8" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I8" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J8" s="106">
         <v>4</v>
@@ -4860,13 +4871,13 @@
         <v>396</v>
       </c>
       <c r="G9" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H9" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I9" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J9" s="106">
         <v>4</v>
@@ -4888,13 +4899,13 @@
         <v>396</v>
       </c>
       <c r="G10" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H10" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I10" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J10" s="106">
         <v>4</v>
@@ -4916,13 +4927,13 @@
         <v>396</v>
       </c>
       <c r="G11" s="106" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H11" s="106" t="s">
         <v>406</v>
       </c>
       <c r="I11" s="106" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J11" s="106">
         <v>4</v>
@@ -4948,7 +4959,7 @@
         <v>318</v>
       </c>
       <c r="G12" s="106" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H12" s="106" t="s">
         <v>416</v>
@@ -4980,7 +4991,7 @@
         <v>322</v>
       </c>
       <c r="G13" s="106" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H13" s="106" t="s">
         <v>416</v>
@@ -5012,7 +5023,7 @@
         <v>318</v>
       </c>
       <c r="G14" s="106" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H14" s="106" t="s">
         <v>416</v>
@@ -5044,7 +5055,7 @@
         <v>322</v>
       </c>
       <c r="G15" s="106" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H15" s="106" t="s">
         <v>416</v>
@@ -5076,13 +5087,13 @@
         <v>302</v>
       </c>
       <c r="G16" s="95" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H16" s="95" t="s">
         <v>406</v>
       </c>
       <c r="I16" s="95" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="J16" s="95"/>
     </row>
@@ -5106,13 +5117,13 @@
         <v>306</v>
       </c>
       <c r="G17" s="95" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H17" s="95" t="s">
         <v>406</v>
       </c>
       <c r="I17" s="95" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="J17" s="95"/>
     </row>
@@ -5136,13 +5147,13 @@
         <v>310</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>406</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="J18" s="24"/>
     </row>
@@ -5166,13 +5177,13 @@
         <v>314</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H19" s="24" t="s">
         <v>406</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="J19" s="24"/>
     </row>
@@ -5194,12 +5205,14 @@
         <v>398</v>
       </c>
       <c r="G20" s="91" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="H20" s="91" t="s">
         <v>406</v>
       </c>
-      <c r="I20" s="91"/>
+      <c r="I20" s="91" t="s">
+        <v>462</v>
+      </c>
       <c r="J20" s="91"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5220,12 +5233,14 @@
         <v>398</v>
       </c>
       <c r="G21" s="92" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="H21" s="92" t="s">
         <v>406</v>
       </c>
-      <c r="I21" s="92"/>
+      <c r="I21" s="92" t="s">
+        <v>462</v>
+      </c>
       <c r="J21" s="92"/>
     </row>
   </sheetData>
@@ -5240,11 +5255,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
@@ -5263,10 +5278,10 @@
         <v>181</v>
       </c>
       <c r="D1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="E1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5280,10 +5295,10 @@
         <v>394</v>
       </c>
       <c r="D2" s="119" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E2" s="119" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5297,10 +5312,10 @@
         <v>394</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E3" s="119" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5314,10 +5329,10 @@
         <v>395</v>
       </c>
       <c r="D4" s="120" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E4" s="120" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5331,10 +5346,10 @@
         <v>395</v>
       </c>
       <c r="D5" s="120" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E5" s="120" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -5348,10 +5363,10 @@
         <v>394</v>
       </c>
       <c r="D6" s="119" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E6" s="119" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5365,10 +5380,10 @@
         <v>394</v>
       </c>
       <c r="D7" s="119" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E7" s="119" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -5382,10 +5397,10 @@
         <v>396</v>
       </c>
       <c r="D8" s="121" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E8" s="121" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -5399,10 +5414,10 @@
         <v>396</v>
       </c>
       <c r="D9" s="121" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E9" s="121" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5415,11 +5430,11 @@
       <c r="C10" s="63" t="s">
         <v>340</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>456</v>
+      <c r="D10" s="121" t="s">
+        <v>449</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5433,10 +5448,10 @@
         <v>341</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -5450,10 +5465,10 @@
         <v>342</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5467,10 +5482,10 @@
         <v>342</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5482,10 +5497,10 @@
       </c>
       <c r="C14" s="122"/>
       <c r="D14" s="122" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E14" s="122" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -5497,10 +5512,10 @@
       </c>
       <c r="C15" s="122"/>
       <c r="D15" s="122" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E15" s="122" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -5514,10 +5529,10 @@
         <v>343</v>
       </c>
       <c r="D16" s="123" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E16" s="123" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -5531,10 +5546,10 @@
         <v>344</v>
       </c>
       <c r="D17" s="123" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E17" s="123" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -5548,10 +5563,10 @@
         <v>345</v>
       </c>
       <c r="D18" s="119" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E18" s="119" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -5565,10 +5580,10 @@
         <v>347</v>
       </c>
       <c r="D19" s="119" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E19" s="119" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -5582,10 +5597,10 @@
         <v>346</v>
       </c>
       <c r="D20" s="124" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E20" s="124" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -5599,10 +5614,10 @@
         <v>348</v>
       </c>
       <c r="D21" s="124" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E21" s="124" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -5616,10 +5631,10 @@
         <v>349</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E22" s="64" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -5633,10 +5648,10 @@
         <v>350</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E23" s="64" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -5650,7 +5665,7 @@
         <v>353</v>
       </c>
       <c r="D24" s="125" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E24" s="125" t="s">
         <v>416</v>
@@ -5667,7 +5682,7 @@
         <v>354</v>
       </c>
       <c r="D25" s="125" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E25" s="125" t="s">
         <v>416</v>
@@ -5684,7 +5699,7 @@
         <v>355</v>
       </c>
       <c r="D26" s="57" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E26" s="57" t="s">
         <v>416</v>
@@ -5701,7 +5716,7 @@
         <v>356</v>
       </c>
       <c r="D27" s="57" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E27" s="57" t="s">
         <v>416</v>
@@ -5718,7 +5733,7 @@
         <v>357</v>
       </c>
       <c r="D28" s="126" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E28" s="126" t="s">
         <v>416</v>
@@ -5735,7 +5750,7 @@
         <v>358</v>
       </c>
       <c r="D29" s="126" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E29" s="126" t="s">
         <v>416</v>
@@ -5752,7 +5767,7 @@
         <v>359</v>
       </c>
       <c r="D30" s="127" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E30" s="127" t="s">
         <v>416</v>
@@ -5769,7 +5784,7 @@
         <v>360</v>
       </c>
       <c r="D31" s="127" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E31" s="127" t="s">
         <v>416</v>
@@ -5786,10 +5801,10 @@
         <v>339</v>
       </c>
       <c r="D32" s="128" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E32" s="128" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -5803,10 +5818,10 @@
         <v>364</v>
       </c>
       <c r="D33" s="128" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E33" s="128" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -5820,10 +5835,10 @@
         <v>396</v>
       </c>
       <c r="D34" s="129" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E34" s="129" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -5837,10 +5852,10 @@
         <v>396</v>
       </c>
       <c r="D35" s="130" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E35" s="130" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -5854,10 +5869,10 @@
         <v>363</v>
       </c>
       <c r="D36" s="129" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="E36" s="129" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -5869,10 +5884,10 @@
       </c>
       <c r="C37" s="118"/>
       <c r="D37" s="148" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="E37" s="148" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -5884,10 +5899,10 @@
       </c>
       <c r="C38" s="116"/>
       <c r="D38" s="149" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="E38" s="149" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -5913,8 +5928,12 @@
       <c r="C40" s="102" t="s">
         <v>361</v>
       </c>
-      <c r="D40" s="151"/>
-      <c r="E40" s="151"/>
+      <c r="D40" s="151" t="s">
+        <v>454</v>
+      </c>
+      <c r="E40" s="151" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="101" t="s">
@@ -5926,8 +5945,12 @@
       <c r="C41" s="102" t="s">
         <v>362</v>
       </c>
-      <c r="D41" s="151"/>
-      <c r="E41" s="151"/>
+      <c r="D41" s="151" t="s">
+        <v>454</v>
+      </c>
+      <c r="E41" s="151" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="103" t="s">
@@ -5939,8 +5962,12 @@
       <c r="C42" s="104" t="s">
         <v>357</v>
       </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="131"/>
+      <c r="D42" s="131" t="s">
+        <v>454</v>
+      </c>
+      <c r="E42" s="131" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="103" t="s">
@@ -5952,8 +5979,12 @@
       <c r="C43" s="131" t="s">
         <v>358</v>
       </c>
-      <c r="D43" s="131"/>
-      <c r="E43" s="131"/>
+      <c r="D43" s="131" t="s">
+        <v>454</v>
+      </c>
+      <c r="E43" s="131" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="105" t="s">
@@ -5965,8 +5996,12 @@
       <c r="C44" s="106" t="s">
         <v>351</v>
       </c>
-      <c r="D44" s="152"/>
-      <c r="E44" s="152"/>
+      <c r="D44" s="152" t="s">
+        <v>454</v>
+      </c>
+      <c r="E44" s="152" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
@@ -5987,7 +6022,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>

</xml_diff>